<commit_message>
updated and moved cycle_path_subgraph input files and proofs
</commit_message>
<xml_diff>
--- a/ontologies/most/experiments/most_group_experiments.xlsx
+++ b/ontologies/most/experiments/most_group_experiments.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/most/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8958CB92-4945-E24F-8043-C34347F83139}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD814E83-8E96-544C-B0A8-8629E8D84409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="most_group2cycle_path_subgraph" sheetId="1" r:id="rId1"/>
     <sheet name="cycle_path_subgraph2most_group" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cycle_path_subgraph2most_group!$A$1:$L$91</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_group2cycle_path_subgraph!$A$1:$L$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cycle_path_subgraph2most_group!$A$1:$L$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_group2cycle_path_subgraph!$A$1:$L$69</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,12 @@
   <si>
     <t>(all x all y all z (betweenMol(x,y,z) -&gt; atom(x) &amp; atom(y) &amp; atom(z))).</t>
   </si>
+  <si>
+    <t>(all a1 all a2 all a3 all a4 all b1 all b2 all g (atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; group(g) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; mol(a3,b2) &amp; mol(a4,b2) &amp; a1 != a3 &amp; a2 != a4 -&gt; mol(b2,g))).</t>
+  </si>
+  <si>
+    <t>(all a1 all a2 all a3 all a4 all g all b1 all b2 all b3 (group(g) &amp; atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; mol(a1,g) &amp; mol(a2,g) &amp; mol(a3,g) &amp; mol(a4,g) &amp; bond(b1) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; bond(b2) &amp; mol(b2,g) &amp; mol(a1,b2) &amp; mol(a3,b2) &amp; bond(b3) &amp; mol(b3,g) &amp; mol(a1,b3) &amp; mol(a4,b3) -&gt; a4 = a3 | a2 = a3 | a4 = a2)).</t>
+  </si>
 </sst>
 </file>
 
@@ -304,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,12 +357,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -860,10 +917,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2540,7 +2597,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_17.proof}</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>43393</v>
       </c>
@@ -2589,7 +2646,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_1,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#1 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_1.proof}</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>43393</v>
       </c>
@@ -2638,7 +2695,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_2,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#2 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_2.proof}</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>43393</v>
       </c>
@@ -2687,7 +2744,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_3,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#3 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_3.proof}</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>43393</v>
       </c>
@@ -2736,7 +2793,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_4,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#4 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_4.proof}</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>43393</v>
       </c>
@@ -2785,7 +2842,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_5,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#5 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_5.proof}</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>43393</v>
       </c>
@@ -2834,7 +2891,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_6,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#6 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_6.proof}</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>43393</v>
       </c>
@@ -2883,7 +2940,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_7,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#7 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_7.proof}</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>43393</v>
       </c>
@@ -2932,7 +2989,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_8,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#8 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_8.proof}</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43393</v>
       </c>
@@ -2981,7 +3038,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_9,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#9 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_9.proof}</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>43393</v>
       </c>
@@ -3030,7 +3087,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_10,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#10 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_10.proof}</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>43393</v>
       </c>
@@ -3079,7 +3136,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_11,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#11 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_11.proof}</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>43393</v>
       </c>
@@ -3128,7 +3185,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_12,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#12 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_12.proof}</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>43393</v>
       </c>
@@ -3177,7 +3234,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_13,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#13 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_13.proof}</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>43393</v>
       </c>
@@ -3226,7 +3283,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_14,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#14 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_14.proof}</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>43393</v>
       </c>
@@ -3275,7 +3332,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_15,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#15 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_15.proof}</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>43393</v>
       </c>
@@ -3324,7 +3381,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_16,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#16 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_16.proof}</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>43393</v>
       </c>
@@ -3373,41 +3430,884 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_17.proof}</v>
       </c>
     </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f>TEXT(A53,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <f>I53&amp;"2"&amp;J53&amp;"_"&amp;C53</f>
+        <v>most_group2cycle_path_subgraph_1</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="3">
+        <v>60</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="3">
+        <v>60</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="1" t="str">
+        <f>I53&amp;"2"&amp;J53</f>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" s="8" t="str">
+        <f>L53&amp;" %"&amp;C53</f>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %1</v>
+      </c>
+      <c r="N53" s="8" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D53&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C53&amp;" in $T_{cycle\_path\_subgraph}$]{proofs/"&amp;D53&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_1,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#1 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_1.proof}</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" ref="B54:B69" si="17">TEXT(A54,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f t="shared" ref="D54:D69" si="18">I54&amp;"2"&amp;J54&amp;"_"&amp;C54</f>
+        <v>most_group2cycle_path_subgraph_2</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="3">
+        <v>60</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="3">
+        <v>60</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="1" t="str">
+        <f t="shared" ref="K54:K69" si="19">I54&amp;"2"&amp;J54</f>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L54" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M54" s="8" t="str">
+        <f>L54&amp;" %"&amp;C54</f>
+        <v>(all x (point(x) | line(x) | plane(x) -&gt; in(x,x))). %2</v>
+      </c>
+      <c r="N54" s="8" t="str">
+        <f t="shared" ref="N54:N69" si="20">"\lstinputlisting[style=p9proof,label="&amp;D54&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C54&amp;" in $T_{cycle\_path\_subgraph}$]{proofs/"&amp;D54&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_2,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#2 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_2.proof}</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_3</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="3">
+        <v>60</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="3">
+        <v>60</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K55" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M55" s="8" t="str">
+        <f>L55&amp;" %"&amp;C55</f>
+        <v>(all p (point(p) -&gt; -line(p))). %3</v>
+      </c>
+      <c r="N55" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_3,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#3 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_3.proof}</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_4</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="3">
+        <v>60</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="3">
+        <v>60</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K56" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" s="8" t="str">
+        <f>L56&amp;" %"&amp;C56</f>
+        <v>(all p (point(p) -&gt; -plane(p))). %4</v>
+      </c>
+      <c r="N56" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_4,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#4 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_4.proof}</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C57" s="1">
+        <v>5</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_5</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="3">
+        <v>60</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57" s="3">
+        <v>60</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M57" s="8" t="str">
+        <f>L57&amp;" %"&amp;C57</f>
+        <v>(all p (plane(p) -&gt; -line(p))). %5</v>
+      </c>
+      <c r="N57" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_5,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#5 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_5.proof}</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C58" s="1">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_6</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="3">
+        <v>60</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" s="3">
+        <v>60</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K58" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L58" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="8" t="str">
+        <f>L58&amp;" %"&amp;C58</f>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %6</v>
+      </c>
+      <c r="N58" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_6,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#6 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_6.proof}</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C59" s="1">
+        <v>7</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_7</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="3">
+        <v>60</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="3">
+        <v>60</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K59" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L59" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="8" t="str">
+        <f>L59&amp;" %"&amp;C59</f>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %7</v>
+      </c>
+      <c r="N59" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_7,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#7 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_7.proof}</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C60" s="1">
+        <v>8</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_8</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="3">
+        <v>60</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H60" s="3">
+        <v>60</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K60" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M60" s="8" t="str">
+        <f>L60&amp;" %"&amp;C60</f>
+        <v>(all x all y (in(x,y) &amp; plane(x) &amp; plane(y) -&gt; x = y)). %8</v>
+      </c>
+      <c r="N60" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_8,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#8 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_8.proof}</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C61" s="1">
+        <v>9</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_9</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="3">
+        <v>60</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H61" s="3">
+        <v>60</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L61" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M61" s="8" t="str">
+        <f>L61&amp;" %"&amp;C61</f>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %9</v>
+      </c>
+      <c r="N61" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_9,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#9 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_9.proof}</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C62" s="1">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_10</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="3">
+        <v>60</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H62" s="3">
+        <v>60</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K62" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L62" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M62" s="8" t="str">
+        <f>L62&amp;" %"&amp;C62</f>
+        <v>(all x (point(x) | line(x) -&gt; in(x,x))). %10</v>
+      </c>
+      <c r="N62" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_10,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#10 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_10.proof}</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C63" s="1">
+        <v>11</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_11</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="3">
+        <v>60</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="3">
+        <v>60</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K63" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L63" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M63" s="8" t="str">
+        <f>L63&amp;" %"&amp;C63</f>
+        <v>(all p (point(p) -&gt; -line(p))). %11</v>
+      </c>
+      <c r="N63" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_11,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#11 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_11.proof}</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C64" s="1">
+        <v>12</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_12</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="3">
+        <v>60</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="3">
+        <v>60</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K64" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L64" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M64" s="8" t="str">
+        <f>L64&amp;" %"&amp;C64</f>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %12</v>
+      </c>
+      <c r="N64" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_12,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#12 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_12.proof}</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C65" s="1">
+        <v>13</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_13</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="3">
+        <v>60</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="3">
+        <v>60</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K65" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L65" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M65" s="8" t="str">
+        <f>L65&amp;" %"&amp;C65</f>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %13</v>
+      </c>
+      <c r="N65" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_13,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#13 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_13.proof}</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C66" s="1">
+        <v>14</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_14</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="3">
+        <v>60</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="3">
+        <v>60</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K66" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L66" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M66" s="8" t="str">
+        <f>L66&amp;" %"&amp;C66</f>
+        <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %14</v>
+      </c>
+      <c r="N66" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_14,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#14 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_14.proof}</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C67" s="1">
+        <v>15</v>
+      </c>
+      <c r="D67" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_15</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="3">
+        <v>60</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H67" s="3">
+        <v>60</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K67" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L67" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M67" s="8" t="str">
+        <f>L67&amp;" %"&amp;C67</f>
+        <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %15</v>
+      </c>
+      <c r="N67" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_15,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#15 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_15.proof}</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C68" s="1">
+        <v>16</v>
+      </c>
+      <c r="D68" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_16</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="3">
+        <v>60</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" s="3">
+        <v>60</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L68" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M68" s="8" t="str">
+        <f>L68&amp;" %"&amp;C68</f>
+        <v>(all x all y all z (plane(x) &amp; line(y) &amp; point(z) &amp; in(z,y) &amp; in(y,x) -&gt; in(z,x))). %16</v>
+      </c>
+      <c r="N68" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_16,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#16 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_16.proof}</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
+        <v>43396</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C69" s="1">
+        <v>17</v>
+      </c>
+      <c r="D69" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>most_group2cycle_path_subgraph_17</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="3">
+        <v>60</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" s="3">
+        <v>60</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K69" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>most_group2cycle_path_subgraph</v>
+      </c>
+      <c r="L69" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M69" s="8" t="str">
+        <f>L69&amp;" %"&amp;C69</f>
+        <v>(all q (plane(q) -&gt; (exists p (point(p) &amp; in(p,q))))). %17</v>
+      </c>
+      <c r="N69" s="8" t="str">
+        <f t="shared" si="20"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_17.proof}</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L52" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L69" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="20" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="10" day="23" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E18">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G18">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E35">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G35">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E52">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G52">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53:E69">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G53:G69">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3419,10 +4319,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996D9C58-6018-1D42-9792-6063C3F60A8A}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N91" sqref="N78:N91"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7064,7 +7964,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_14,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#14 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_14.proof}</v>
       </c>
     </row>
-    <row r="78" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
         <v>43393</v>
       </c>
@@ -7113,7 +8013,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_1,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#1 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_1.proof}</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9">
         <v>43393</v>
       </c>
@@ -7162,7 +8062,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_2,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#2 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_2.proof}</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9">
         <v>43393</v>
       </c>
@@ -7211,7 +8111,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_3,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#3 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_3.proof}</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9">
         <v>43393</v>
       </c>
@@ -7260,7 +8160,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_4,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#4 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_4.proof}</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
         <v>43393</v>
       </c>
@@ -7309,7 +8209,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_5,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#5 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_5.proof}</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9">
         <v>43393</v>
       </c>
@@ -7358,7 +8258,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_6,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#6 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_6.proof}</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
         <v>43393</v>
       </c>
@@ -7407,7 +8307,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_7,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#7 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_7.proof}</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
         <v>43393</v>
       </c>
@@ -7456,7 +8356,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_8,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#8 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_8.proof}</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
         <v>43393</v>
       </c>
@@ -7505,7 +8405,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_9,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#9 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_9.proof}</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
         <v>43393</v>
       </c>
@@ -7554,7 +8454,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_10,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#10 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_10.proof}</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="9">
         <v>43393</v>
       </c>
@@ -7603,7 +8503,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_11,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#11 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_11.proof}</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9">
         <v>43393</v>
       </c>
@@ -7652,7 +8552,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_12,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#12 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_12.proof}</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9">
         <v>43393</v>
       </c>
@@ -7701,7 +8601,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_13,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#13 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_13.proof}</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="9">
         <v>43393</v>
       </c>
@@ -7750,50 +8650,746 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_14,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#14 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_14.proof}</v>
       </c>
     </row>
+    <row r="92" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="9">
+        <v>43396</v>
+      </c>
+      <c r="B92" s="10" t="str">
+        <f>TEXT(A92,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C92" s="10">
+        <v>1</v>
+      </c>
+      <c r="D92" s="10" t="str">
+        <f t="shared" ref="D92:D105" si="24">I92&amp;"2"&amp;J92&amp;"_"&amp;C92</f>
+        <v>cycle_path_subgraph2most_group_1</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="12">
+        <v>60</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" s="12">
+        <v>60</v>
+      </c>
+      <c r="I92" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K92" s="10" t="str">
+        <f t="shared" ref="K92:K105" si="25">I92&amp;"2"&amp;J92</f>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L92" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M92" s="13" t="str">
+        <f>L92&amp;" %"&amp;C92</f>
+        <v>(all x (atom(x) -&gt; -(bond(x) | group(x)))). %1</v>
+      </c>
+      <c r="N92" s="13" t="str">
+        <f t="shared" ref="N92:N105" si="26">"\lstinputlisting[style=p9proof,label="&amp;D92&amp;",caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#"&amp;C92&amp;" in $T_{most\_group}$]{proofs/"&amp;D92&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_1,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#1 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_1.proof}</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f t="shared" ref="B93:B105" si="27">TEXT(A93,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2</v>
+      </c>
+      <c r="D93" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_2</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="3">
+        <v>60</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" s="3">
+        <v>60</v>
+      </c>
+      <c r="I93" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K93" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L93" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M93" s="15" t="str">
+        <f t="shared" ref="M93:M105" si="28">L93&amp;" %"&amp;C93</f>
+        <v>(all x (bond(x) -&gt; -group(x))). %2</v>
+      </c>
+      <c r="N93" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_2,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#2 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_2.proof}</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C94" s="1">
+        <v>3</v>
+      </c>
+      <c r="D94" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_3</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="3">
+        <v>60</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" s="3">
+        <v>60</v>
+      </c>
+      <c r="I94" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K94" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L94" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M94" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x all y (mol(x,y) &amp; group(x) &amp; group(y) -&gt; x = y)). %3</v>
+      </c>
+      <c r="N94" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_3,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#3 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_3.proof}</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C95" s="1">
+        <v>4</v>
+      </c>
+      <c r="D95" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_4</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="3">
+        <v>60</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" s="3">
+        <v>60</v>
+      </c>
+      <c r="I95" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J95" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K95" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L95" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M95" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x (group(x) -&gt; (exists a (atom(a) &amp; mol(a,x))))). %4</v>
+      </c>
+      <c r="N95" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_4,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#4 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_4.proof}</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C96" s="1">
+        <v>5</v>
+      </c>
+      <c r="D96" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_5</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="3">
+        <v>60</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" s="3">
+        <v>60</v>
+      </c>
+      <c r="I96" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J96" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K96" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L96" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M96" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x (atom(x) -&gt; (exists y (group(y) &amp; mol(x,y))))). %5</v>
+      </c>
+      <c r="N96" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_5,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#5 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_5.proof}</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C97" s="1">
+        <v>6</v>
+      </c>
+      <c r="D97" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_6</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="3">
+        <v>60</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H97" s="3">
+        <v>60</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J97" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K97" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L97" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M97" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x (atom(x) -&gt; (exists b exists y exists z (bond(b) &amp; group(y) &amp; atom(z) &amp; x != z &amp; mol(x,b) &amp; mol(z,b) &amp; mol(z,y))))). %6</v>
+      </c>
+      <c r="N97" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_6,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#6 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_6.proof}</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C98" s="1">
+        <v>7</v>
+      </c>
+      <c r="D98" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_7</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="3">
+        <v>60</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" s="3">
+        <v>60</v>
+      </c>
+      <c r="I98" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J98" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K98" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L98" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M98" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all b all g all x all y (atom(x) &amp; atom(y) &amp; x != y &amp; bond(b) &amp; group(g) &amp; mol(x,b) &amp; mol(y,b) &amp; mol(b,g) -&gt; mol(x,g))). %7</v>
+      </c>
+      <c r="N98" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_7,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#7 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_7.proof}</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C99" s="1">
+        <v>8</v>
+      </c>
+      <c r="D99" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_8</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="3">
+        <v>60</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" s="3">
+        <v>60</v>
+      </c>
+      <c r="I99" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J99" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K99" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L99" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M99" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x all y all z (atom(x) &amp; bond(y) &amp; group(z) &amp; mol(x,y) &amp; mol(y,z) -&gt; mol(x,z))). %8</v>
+      </c>
+      <c r="N99" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_8,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#8 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_8.proof}</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B100" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C100" s="1">
+        <v>9</v>
+      </c>
+      <c r="D100" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_9</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="3">
+        <v>60</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" s="3">
+        <v>60</v>
+      </c>
+      <c r="I100" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J100" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K100" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L100" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M100" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all a1 all a2 all a3 all a4 all b1 all b2 all g (atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; group(g) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; mol(a3,b2) &amp; mol(a4,b2) &amp; a1 != a3 &amp; a2 != a4 -&gt; mol(b2,g))). %9</v>
+      </c>
+      <c r="N100" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_9,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#9 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_9.proof}</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B101" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C101" s="1">
+        <v>10</v>
+      </c>
+      <c r="D101" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_10</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="3">
+        <v>60</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="3">
+        <v>60</v>
+      </c>
+      <c r="I101" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K101" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L101" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M101" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all y (group(y) -&gt; (exists x (atom(x) &amp; mol(x,y))))). %10</v>
+      </c>
+      <c r="N101" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_10,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#10 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_10.proof}</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B102" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C102" s="1">
+        <v>11</v>
+      </c>
+      <c r="D102" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_11</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="3">
+        <v>60</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H102" s="3">
+        <v>60</v>
+      </c>
+      <c r="I102" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J102" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K102" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L102" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M102" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x all y all b all g (atom(x) &amp; atom(y) &amp; bond(b) &amp; group(g) &amp; x != y &amp; mol(x,y) &amp; mol(y,g) &amp; mol(x,b) &amp; mol(y,b) -&gt; mol(b,g))). %11</v>
+      </c>
+      <c r="N102" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_11,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#11 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_11.proof}</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C103" s="1">
+        <v>12</v>
+      </c>
+      <c r="D103" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_12</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" s="3">
+        <v>60</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="3">
+        <v>60</v>
+      </c>
+      <c r="I103" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J103" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K103" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L103" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M103" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all b all g (bond(b) &amp; group(g) &amp; -mol(b,g) -&gt; (exists a (atom(a) &amp; mol(a,b) &amp; -mol(a,g))))). %12</v>
+      </c>
+      <c r="N103" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_12,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#12 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_12.proof}</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A104" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B104" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C104" s="1">
+        <v>13</v>
+      </c>
+      <c r="D104" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_13</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" s="3">
+        <v>60</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" s="3">
+        <v>60</v>
+      </c>
+      <c r="I104" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J104" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K104" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L104" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M104" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all x all y all z all w (group(x) &amp; end(y,x) &amp; end(z,x) &amp; end(w,x) -&gt; y = z | y = w | z = w)). %13</v>
+      </c>
+      <c r="N104" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_13,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#13 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_13.proof}</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" s="16">
+        <v>43396</v>
+      </c>
+      <c r="B105" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1023_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C105" s="1">
+        <v>14</v>
+      </c>
+      <c r="D105" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>cycle_path_subgraph2most_group_14</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="3">
+        <v>60</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="3">
+        <v>60</v>
+      </c>
+      <c r="I105" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J105" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K105" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>cycle_path_subgraph2most_group</v>
+      </c>
+      <c r="L105" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="M105" s="15" t="str">
+        <f t="shared" si="28"/>
+        <v>(all a1 all a2 all a3 all a4 all g all b1 all b2 all b3 (group(g) &amp; atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; mol(a1,g) &amp; mol(a2,g) &amp; mol(a3,g) &amp; mol(a4,g) &amp; bond(b1) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; bond(b2) &amp; mol(b2,g) &amp; mol(a1,b2) &amp; mol(a3,b2) &amp; bond(b3) &amp; mol(b3,g) &amp; mol(a1,b3) &amp; mol(a4,b3) -&gt; a4 = a3 | a2 = a3 | a4 = a2)). %14</v>
+      </c>
+      <c r="N105" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_14,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#14 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_14.proof}</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L91" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L105" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="20" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="10" day="23" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E49">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G49">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E63">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G50:G63">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E63">
+  <conditionalFormatting sqref="E64:E77">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G63">
+  <conditionalFormatting sqref="G64:G77">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:E77">
+  <conditionalFormatting sqref="E78:E91">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G64:G77">
+  <conditionalFormatting sqref="G78:G91">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78:E91">
+  <conditionalFormatting sqref="E92:E105">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G78:G91">
+  <conditionalFormatting sqref="G92:G105">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated and moved most_group2cycle_path_subgraph input files and proofs
</commit_message>
<xml_diff>
--- a/ontologies/most/experiments/most_group_experiments.xlsx
+++ b/ontologies/most/experiments/most_group_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/most/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD814E83-8E96-544C-B0A8-8629E8D84409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2244CF75-A07A-EB4D-8E35-A80BE4EBCD85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="most_group2cycle_path_subgraph" sheetId="1" r:id="rId1"/>
@@ -919,8 +919,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M69" sqref="M53:M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4321,8 +4321,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView topLeftCell="C1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated most experiment files
</commit_message>
<xml_diff>
--- a/ontologies/most/experiments/most_group_experiments.xlsx
+++ b/ontologies/most/experiments/most_group_experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/most/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2244CF75-A07A-EB4D-8E35-A80BE4EBCD85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFD857B-87F9-D943-AE09-7C2C6952ABF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,15 @@
     <sheet name="cycle_path_subgraph2most_group" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cycle_path_subgraph2most_group!$A$1:$L$105</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_group2cycle_path_subgraph!$A$1:$L$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cycle_path_subgraph2most_group!$A$1:$L$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_group2cycle_path_subgraph!$A$1:$L$86</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -221,6 +221,30 @@
   <si>
     <t>(all a1 all a2 all a3 all a4 all g all b1 all b2 all b3 (group(g) &amp; atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; mol(a1,g) &amp; mol(a2,g) &amp; mol(a3,g) &amp; mol(a4,g) &amp; bond(b1) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; bond(b2) &amp; mol(b2,g) &amp; mol(a1,b2) &amp; mol(a3,b2) &amp; bond(b3) &amp; mol(b3,g) &amp; mol(a1,b3) &amp; mol(a4,b3) -&gt; a4 = a3 | a2 = a3 | a4 = a2)).</t>
   </si>
+  <si>
+    <t>cycle_path_subgraph_nonisolated</t>
+  </si>
+  <si>
+    <t>make sure to comment out definitions</t>
+  </si>
+  <si>
+    <t>(all x all y all z all w all q all l1 all l2 all l3 (plane(q) &amp; point(x) &amp; point(y) &amp; point(z) &amp; point(w) &amp; in(x,q) &amp; in(y,q) &amp; in(z,q) &amp; in(w,q) &amp; line(l1) &amp; in(l1,q) &amp; in(x,l1) &amp; in(y,l1) &amp; line(l2) &amp; in(l2,q) &amp; in(x,l2) &amp; in(z,l2) &amp; line(l3) &amp; in(l3,q) &amp; in(x,l3) &amp; in(w,l3) -&gt; w = z | y = z | w = y)).</t>
+  </si>
+  <si>
+    <t>(all q all x all y all z (planar_pendant(x,q) &amp; planar_pendant(y,q) &amp; planar_pendant(z,q) -&gt; x = y | y = z | z = x)).</t>
+  </si>
+  <si>
+    <t>(all p (point(p) -&gt; (exists l (line(l) &amp; in(p,l))))).</t>
+  </si>
+  <si>
+    <t>(all l all q (line(l) &amp; plane(q) &amp; -in(l,q) -&gt; (exists p (point(p) &amp; in(p,l) &amp; -in(p,q))))).</t>
+  </si>
+  <si>
+    <t>(all l (line(l) -&gt; (exists x exists y (point(x) &amp; point(y) &amp; x != y &amp; in(x,l) &amp; in(y,l))))).</t>
+  </si>
+  <si>
+    <t>(all p (point(p) -&gt; (exists q (plane(q) &amp; in(p,q))))).</t>
+  </si>
 </sst>
 </file>
 
@@ -250,7 +274,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -305,12 +335,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,12 +399,81 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -917,10 +1025,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M69" sqref="M53:M69"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P98" sqref="P98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3430,7 +3538,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_17.proof}</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>43396</v>
       </c>
@@ -3471,7 +3579,7 @@
         <v>16</v>
       </c>
       <c r="M53" s="8" t="str">
-        <f>L53&amp;" %"&amp;C53</f>
+        <f t="shared" ref="M53:M69" si="17">L53&amp;" %"&amp;C53</f>
         <v>(all x all y (in(x,y) -&gt; in(y,x))). %1</v>
       </c>
       <c r="N53" s="8" t="str">
@@ -3479,19 +3587,19 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_1,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#1 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_1.proof}</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>43396</v>
       </c>
       <c r="B54" s="1" t="str">
-        <f t="shared" ref="B54:B69" si="17">TEXT(A54,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <f t="shared" ref="B54:B69" si="18">TEXT(A54,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C54" s="1">
         <v>2</v>
       </c>
       <c r="D54" s="1" t="str">
-        <f t="shared" ref="D54:D69" si="18">I54&amp;"2"&amp;J54&amp;"_"&amp;C54</f>
+        <f t="shared" ref="D54:D69" si="19">I54&amp;"2"&amp;J54&amp;"_"&amp;C54</f>
         <v>most_group2cycle_path_subgraph_2</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -3513,34 +3621,34 @@
         <v>23</v>
       </c>
       <c r="K54" s="1" t="str">
-        <f t="shared" ref="K54:K69" si="19">I54&amp;"2"&amp;J54</f>
+        <f t="shared" ref="K54:K69" si="20">I54&amp;"2"&amp;J54</f>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M54" s="8" t="str">
-        <f>L54&amp;" %"&amp;C54</f>
+        <f t="shared" si="17"/>
         <v>(all x (point(x) | line(x) | plane(x) -&gt; in(x,x))). %2</v>
       </c>
       <c r="N54" s="8" t="str">
-        <f t="shared" ref="N54:N69" si="20">"\lstinputlisting[style=p9proof,label="&amp;D54&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C54&amp;" in $T_{cycle\_path\_subgraph}$]{proofs/"&amp;D54&amp;".proof}"</f>
+        <f t="shared" ref="N54:N69" si="21">"\lstinputlisting[style=p9proof,label="&amp;D54&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C54&amp;" in $T_{cycle\_path\_subgraph}$]{proofs/"&amp;D54&amp;".proof}"</f>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_2,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#2 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_2.proof}</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>43396</v>
       </c>
       <c r="B55" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C55" s="1">
         <v>3</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_3</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -3562,34 +3670,34 @@
         <v>23</v>
       </c>
       <c r="K55" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>18</v>
       </c>
       <c r="M55" s="8" t="str">
-        <f>L55&amp;" %"&amp;C55</f>
+        <f t="shared" si="17"/>
         <v>(all p (point(p) -&gt; -line(p))). %3</v>
       </c>
       <c r="N55" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_3,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#3 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_3.proof}</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>43396</v>
       </c>
       <c r="B56" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_4</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -3611,34 +3719,34 @@
         <v>23</v>
       </c>
       <c r="K56" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L56" s="8" t="s">
         <v>25</v>
       </c>
       <c r="M56" s="8" t="str">
-        <f>L56&amp;" %"&amp;C56</f>
+        <f t="shared" si="17"/>
         <v>(all p (point(p) -&gt; -plane(p))). %4</v>
       </c>
       <c r="N56" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_4,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#4 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_4.proof}</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>43396</v>
       </c>
       <c r="B57" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C57" s="1">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_5</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -3660,34 +3768,34 @@
         <v>23</v>
       </c>
       <c r="K57" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L57" s="8" t="s">
         <v>26</v>
       </c>
       <c r="M57" s="8" t="str">
-        <f>L57&amp;" %"&amp;C57</f>
+        <f t="shared" si="17"/>
         <v>(all p (plane(p) -&gt; -line(p))). %5</v>
       </c>
       <c r="N57" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_5,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#5 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_5.proof}</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>43396</v>
       </c>
       <c r="B58" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C58" s="1">
         <v>6</v>
       </c>
       <c r="D58" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_6</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -3709,34 +3817,34 @@
         <v>23</v>
       </c>
       <c r="K58" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L58" s="8" t="s">
         <v>19</v>
       </c>
       <c r="M58" s="8" t="str">
-        <f>L58&amp;" %"&amp;C58</f>
+        <f t="shared" si="17"/>
         <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %6</v>
       </c>
       <c r="N58" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_6,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#6 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_6.proof}</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>43396</v>
       </c>
       <c r="B59" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C59" s="1">
         <v>7</v>
       </c>
       <c r="D59" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_7</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -3758,34 +3866,34 @@
         <v>23</v>
       </c>
       <c r="K59" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L59" s="8" t="s">
         <v>20</v>
       </c>
       <c r="M59" s="8" t="str">
-        <f>L59&amp;" %"&amp;C59</f>
+        <f t="shared" si="17"/>
         <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %7</v>
       </c>
       <c r="N59" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_7,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#7 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_7.proof}</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>43396</v>
       </c>
       <c r="B60" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C60" s="1">
         <v>8</v>
       </c>
       <c r="D60" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_8</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -3807,34 +3915,34 @@
         <v>23</v>
       </c>
       <c r="K60" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>27</v>
       </c>
       <c r="M60" s="8" t="str">
-        <f>L60&amp;" %"&amp;C60</f>
+        <f t="shared" si="17"/>
         <v>(all x all y (in(x,y) &amp; plane(x) &amp; plane(y) -&gt; x = y)). %8</v>
       </c>
       <c r="N60" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_8,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#8 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_8.proof}</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>43396</v>
       </c>
       <c r="B61" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C61" s="1">
         <v>9</v>
       </c>
       <c r="D61" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_9</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -3856,34 +3964,34 @@
         <v>23</v>
       </c>
       <c r="K61" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L61" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M61" s="8" t="str">
-        <f>L61&amp;" %"&amp;C61</f>
+        <f t="shared" si="17"/>
         <v>(all x all y (in(x,y) -&gt; in(y,x))). %9</v>
       </c>
       <c r="N61" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_9,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#9 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_9.proof}</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>43396</v>
       </c>
       <c r="B62" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C62" s="1">
         <v>10</v>
       </c>
       <c r="D62" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_10</v>
       </c>
       <c r="E62" s="2" t="s">
@@ -3905,34 +4013,34 @@
         <v>23</v>
       </c>
       <c r="K62" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L62" s="8" t="s">
         <v>17</v>
       </c>
       <c r="M62" s="8" t="str">
-        <f>L62&amp;" %"&amp;C62</f>
+        <f t="shared" si="17"/>
         <v>(all x (point(x) | line(x) -&gt; in(x,x))). %10</v>
       </c>
       <c r="N62" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_10,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#10 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_10.proof}</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>43396</v>
       </c>
       <c r="B63" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C63" s="1">
         <v>11</v>
       </c>
       <c r="D63" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_11</v>
       </c>
       <c r="E63" s="2" t="s">
@@ -3954,34 +4062,34 @@
         <v>23</v>
       </c>
       <c r="K63" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L63" s="8" t="s">
         <v>18</v>
       </c>
       <c r="M63" s="8" t="str">
-        <f>L63&amp;" %"&amp;C63</f>
+        <f t="shared" si="17"/>
         <v>(all p (point(p) -&gt; -line(p))). %11</v>
       </c>
       <c r="N63" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_11,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#11 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_11.proof}</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>43396</v>
       </c>
       <c r="B64" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C64" s="1">
         <v>12</v>
       </c>
       <c r="D64" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_12</v>
       </c>
       <c r="E64" s="2" t="s">
@@ -4003,34 +4111,34 @@
         <v>23</v>
       </c>
       <c r="K64" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L64" s="8" t="s">
         <v>19</v>
       </c>
       <c r="M64" s="8" t="str">
-        <f>L64&amp;" %"&amp;C64</f>
+        <f t="shared" si="17"/>
         <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %12</v>
       </c>
       <c r="N64" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_12,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#12 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_12.proof}</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>43396</v>
       </c>
       <c r="B65" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C65" s="1">
         <v>13</v>
       </c>
       <c r="D65" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_13</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -4052,34 +4160,34 @@
         <v>23</v>
       </c>
       <c r="K65" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L65" s="8" t="s">
         <v>20</v>
       </c>
       <c r="M65" s="8" t="str">
-        <f>L65&amp;" %"&amp;C65</f>
+        <f t="shared" si="17"/>
         <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %13</v>
       </c>
       <c r="N65" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_13,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#13 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_13.proof}</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>43396</v>
       </c>
       <c r="B66" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C66" s="1">
         <v>14</v>
       </c>
       <c r="D66" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_14</v>
       </c>
       <c r="E66" s="2" t="s">
@@ -4101,34 +4209,34 @@
         <v>23</v>
       </c>
       <c r="K66" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L66" s="8" t="s">
         <v>14</v>
       </c>
       <c r="M66" s="8" t="str">
-        <f>L66&amp;" %"&amp;C66</f>
+        <f t="shared" si="17"/>
         <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %14</v>
       </c>
       <c r="N66" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_14,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#14 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_14.proof}</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>43396</v>
       </c>
       <c r="B67" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C67" s="1">
         <v>15</v>
       </c>
       <c r="D67" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_15</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -4150,34 +4258,34 @@
         <v>23</v>
       </c>
       <c r="K67" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L67" s="8" t="s">
         <v>15</v>
       </c>
       <c r="M67" s="8" t="str">
-        <f>L67&amp;" %"&amp;C67</f>
+        <f t="shared" si="17"/>
         <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %15</v>
       </c>
       <c r="N67" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_15,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#15 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_15.proof}</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>43396</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C68" s="1">
         <v>16</v>
       </c>
       <c r="D68" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_16</v>
       </c>
       <c r="E68" s="2" t="s">
@@ -4199,34 +4307,34 @@
         <v>23</v>
       </c>
       <c r="K68" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L68" s="8" t="s">
         <v>28</v>
       </c>
       <c r="M68" s="8" t="str">
-        <f>L68&amp;" %"&amp;C68</f>
+        <f t="shared" si="17"/>
         <v>(all x all y all z (plane(x) &amp; line(y) &amp; point(z) &amp; in(z,y) &amp; in(y,x) -&gt; in(z,x))). %16</v>
       </c>
       <c r="N68" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_16,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#16 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_16.proof}</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>43396</v>
       </c>
       <c r="B69" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
       <c r="C69" s="1">
         <v>17</v>
       </c>
       <c r="D69" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>most_group2cycle_path_subgraph_17</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -4248,66 +4356,1215 @@
         <v>23</v>
       </c>
       <c r="K69" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>most_group2cycle_path_subgraph</v>
       </c>
       <c r="L69" s="8" t="s">
         <v>29</v>
       </c>
       <c r="M69" s="8" t="str">
-        <f>L69&amp;" %"&amp;C69</f>
+        <f t="shared" si="17"/>
         <v>(all q (plane(q) -&gt; (exists p (point(p) &amp; in(p,q))))). %17</v>
       </c>
       <c r="N69" s="8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_17.proof}</v>
       </c>
     </row>
+    <row r="70" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B70" s="14" t="str">
+        <f>TEXT(A70,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C70" s="14">
+        <v>1</v>
+      </c>
+      <c r="D70" s="14" t="str">
+        <f>I70&amp;"2"&amp;J70&amp;"_"&amp;C70</f>
+        <v>most_group2cycle_path_subgraph_nonisolated_1</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="3">
+        <v>600</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" s="3">
+        <v>600</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K70" s="14" t="str">
+        <f>I70&amp;"2"&amp;J70</f>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L70" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="M70" s="15" t="str">
+        <f t="shared" ref="M70:M86" si="22">L70&amp;" %"&amp;C70</f>
+        <v>(all x all y all z all w all q all l1 all l2 all l3 (plane(q) &amp; point(x) &amp; point(y) &amp; point(z) &amp; point(w) &amp; in(x,q) &amp; in(y,q) &amp; in(z,q) &amp; in(w,q) &amp; line(l1) &amp; in(l1,q) &amp; in(x,l1) &amp; in(y,l1) &amp; line(l2) &amp; in(l2,q) &amp; in(x,l2) &amp; in(z,l2) &amp; line(l3) &amp; in(l3,q) &amp; in(x,l3) &amp; in(w,l3) -&gt; w = z | y = z | w = y)). %1</v>
+      </c>
+      <c r="N70" s="15" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D70&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C70&amp;" in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/"&amp;D70&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_1,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#1 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_1.proof}</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B71" s="14" t="str">
+        <f t="shared" ref="B71:B86" si="23">TEXT(A71,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C71" s="14">
+        <v>2</v>
+      </c>
+      <c r="D71" s="14" t="str">
+        <f t="shared" ref="D71:D86" si="24">I71&amp;"2"&amp;J71&amp;"_"&amp;C71</f>
+        <v>most_group2cycle_path_subgraph_nonisolated_2</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="3">
+        <v>600</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H71" s="3">
+        <v>600</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K71" s="14" t="str">
+        <f t="shared" ref="K71:K86" si="25">I71&amp;"2"&amp;J71</f>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L71" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="M71" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all q all x all y all z (planar_pendant(x,q) &amp; planar_pendant(y,q) &amp; planar_pendant(z,q) -&gt; x = y | y = z | z = x)). %2</v>
+      </c>
+      <c r="N71" s="15" t="str">
+        <f t="shared" ref="N71:N92" si="26">"\lstinputlisting[style=p9proof,label="&amp;D71&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C71&amp;" in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/"&amp;D71&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_2,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#2 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_2.proof}</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B72" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C72" s="14">
+        <v>3</v>
+      </c>
+      <c r="D72" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_3</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="3">
+        <v>600</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" s="3">
+        <v>600</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J72" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K72" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L72" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="M72" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all p (point(p) -&gt; (exists l (line(l) &amp; in(p,l))))). %3</v>
+      </c>
+      <c r="N72" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_3,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#3 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_3.proof}</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B73" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C73" s="14">
+        <v>4</v>
+      </c>
+      <c r="D73" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_4</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="3">
+        <v>600</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" s="3">
+        <v>600</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K73" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L73" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M73" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all l all q (line(l) &amp; plane(q) &amp; -in(l,q) -&gt; (exists p (point(p) &amp; in(p,l) &amp; -in(p,q))))). %4</v>
+      </c>
+      <c r="N73" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_4,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#4 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_4.proof}</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B74" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C74" s="14">
+        <v>5</v>
+      </c>
+      <c r="D74" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_5</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="3">
+        <v>600</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H74" s="3">
+        <v>600</v>
+      </c>
+      <c r="I74" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K74" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L74" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="M74" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all l (line(l) -&gt; (exists x exists y (point(x) &amp; point(y) &amp; x != y &amp; in(x,l) &amp; in(y,l))))). %5</v>
+      </c>
+      <c r="N74" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_5,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#5 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_5.proof}</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B75" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C75" s="14">
+        <v>6</v>
+      </c>
+      <c r="D75" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_6</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="3">
+        <v>600</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H75" s="3">
+        <v>600</v>
+      </c>
+      <c r="I75" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K75" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L75" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M75" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %6</v>
+      </c>
+      <c r="N75" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_6,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#6 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_6.proof}</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B76" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C76" s="14">
+        <v>7</v>
+      </c>
+      <c r="D76" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_7</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="3">
+        <v>600</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H76" s="3">
+        <v>600</v>
+      </c>
+      <c r="I76" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J76" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K76" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L76" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M76" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x (point(x) | line(x) | plane(x) -&gt; in(x,x))). %7</v>
+      </c>
+      <c r="N76" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_7,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#7 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_7.proof}</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B77" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C77" s="14">
+        <v>8</v>
+      </c>
+      <c r="D77" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_8</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="3">
+        <v>600</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H77" s="3">
+        <v>600</v>
+      </c>
+      <c r="I77" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J77" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K77" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L77" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M77" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all p (point(p) -&gt; -line(p))). %8</v>
+      </c>
+      <c r="N77" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_8,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#8 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_8.proof}</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B78" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C78" s="14">
+        <v>9</v>
+      </c>
+      <c r="D78" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_9</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="3">
+        <v>600</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H78" s="3">
+        <v>600</v>
+      </c>
+      <c r="I78" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J78" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K78" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L78" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M78" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all p (point(p) -&gt; -plane(p))). %9</v>
+      </c>
+      <c r="N78" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_9,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#9 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_9.proof}</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B79" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C79" s="14">
+        <v>10</v>
+      </c>
+      <c r="D79" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_10</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="3">
+        <v>600</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H79" s="3">
+        <v>600</v>
+      </c>
+      <c r="I79" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J79" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K79" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L79" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="M79" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all p (plane(p) -&gt; -line(p))). %10</v>
+      </c>
+      <c r="N79" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_10,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#10 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_10.proof}</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B80" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C80" s="14">
+        <v>11</v>
+      </c>
+      <c r="D80" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_11</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="3">
+        <v>600</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" s="3">
+        <v>600</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J80" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K80" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L80" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M80" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %11</v>
+      </c>
+      <c r="N80" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_11,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#11 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_11.proof}</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B81" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C81" s="14">
+        <v>12</v>
+      </c>
+      <c r="D81" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_12</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="3">
+        <v>600</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H81" s="3">
+        <v>600</v>
+      </c>
+      <c r="I81" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J81" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K81" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L81" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M81" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %12</v>
+      </c>
+      <c r="N81" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_12,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#12 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_12.proof}</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B82" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C82" s="14">
+        <v>13</v>
+      </c>
+      <c r="D82" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_13</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="3">
+        <v>600</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H82" s="3">
+        <v>600</v>
+      </c>
+      <c r="I82" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J82" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K82" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L82" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M82" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x all y (in(x,y) &amp; plane(x) &amp; plane(y) -&gt; x = y)). %13</v>
+      </c>
+      <c r="N82" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_13,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#13 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_13.proof}</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B83" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C83" s="14">
+        <v>14</v>
+      </c>
+      <c r="D83" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_14</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="3">
+        <v>600</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H83" s="3">
+        <v>600</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K83" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L83" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M83" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %14</v>
+      </c>
+      <c r="N83" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_14,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#14 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_14.proof}</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B84" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C84" s="14">
+        <v>15</v>
+      </c>
+      <c r="D84" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_15</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="3">
+        <v>600</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H84" s="3">
+        <v>600</v>
+      </c>
+      <c r="I84" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K84" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L84" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M84" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x (point(x) | line(x) -&gt; in(x,x))). %15</v>
+      </c>
+      <c r="N84" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_15,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#15 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_15.proof}</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B85" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C85" s="14">
+        <v>16</v>
+      </c>
+      <c r="D85" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_16</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="3">
+        <v>600</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H85" s="3">
+        <v>600</v>
+      </c>
+      <c r="I85" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K85" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M85" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all p (point(p) -&gt; -line(p))). %16</v>
+      </c>
+      <c r="N85" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_16,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#16 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_16.proof}</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B86" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C86" s="14">
+        <v>17</v>
+      </c>
+      <c r="D86" s="14" t="str">
+        <f t="shared" si="24"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_17</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="3">
+        <v>600</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H86" s="3">
+        <v>600</v>
+      </c>
+      <c r="I86" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J86" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K86" s="14" t="str">
+        <f t="shared" si="25"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L86" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M86" s="15" t="str">
+        <f t="shared" si="22"/>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %17</v>
+      </c>
+      <c r="N86" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_17.proof}</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A87" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B87" s="14" t="str">
+        <f t="shared" ref="B87:B92" si="27">TEXT(A87,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C87" s="14">
+        <v>18</v>
+      </c>
+      <c r="D87" s="14" t="str">
+        <f t="shared" ref="D87:D92" si="28">I87&amp;"2"&amp;J87&amp;"_"&amp;C87</f>
+        <v>most_group2cycle_path_subgraph_nonisolated_18</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="3">
+        <v>600</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" s="3">
+        <v>600</v>
+      </c>
+      <c r="I87" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J87" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K87" s="14" t="str">
+        <f t="shared" ref="K87:K92" si="29">I87&amp;"2"&amp;J87</f>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L87" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M87" s="15" t="str">
+        <f t="shared" ref="M87:M92" si="30">L87&amp;" %"&amp;C87</f>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %18</v>
+      </c>
+      <c r="N87" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_18,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#18 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_18.proof}</v>
+      </c>
+      <c r="O87" s="14"/>
+      <c r="P87" s="14"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A88" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B88" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C88" s="14">
+        <v>19</v>
+      </c>
+      <c r="D88" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_19</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="3">
+        <v>600</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H88" s="3">
+        <v>600</v>
+      </c>
+      <c r="I88" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J88" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K88" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L88" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="M88" s="15" t="str">
+        <f t="shared" si="30"/>
+        <v>(all p (point(p) -&gt; (exists q (plane(q) &amp; in(p,q))))). %19</v>
+      </c>
+      <c r="N88" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_19,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#19 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_19.proof}</v>
+      </c>
+      <c r="O88" s="14"/>
+      <c r="P88" s="14"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A89" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B89" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C89" s="14">
+        <v>20</v>
+      </c>
+      <c r="D89" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_20</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="3">
+        <v>600</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H89" s="3">
+        <v>600</v>
+      </c>
+      <c r="I89" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J89" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K89" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L89" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M89" s="15" t="str">
+        <f t="shared" si="30"/>
+        <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %20</v>
+      </c>
+      <c r="N89" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_20,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#20 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_20.proof}</v>
+      </c>
+      <c r="O89" s="14"/>
+      <c r="P89" s="14"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A90" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B90" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C90" s="14">
+        <v>21</v>
+      </c>
+      <c r="D90" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_21</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" s="3">
+        <v>600</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H90" s="3">
+        <v>600</v>
+      </c>
+      <c r="I90" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J90" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K90" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L90" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M90" s="15" t="str">
+        <f t="shared" si="30"/>
+        <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %21</v>
+      </c>
+      <c r="N90" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_21,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#21 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_21.proof}</v>
+      </c>
+      <c r="O90" s="14"/>
+      <c r="P90" s="14"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A91" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B91" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C91" s="14">
+        <v>22</v>
+      </c>
+      <c r="D91" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_22</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" s="3">
+        <v>600</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" s="3">
+        <v>600</v>
+      </c>
+      <c r="I91" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J91" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K91" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L91" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M91" s="15" t="str">
+        <f t="shared" si="30"/>
+        <v>(all x all y all z (plane(x) &amp; line(y) &amp; point(z) &amp; in(z,y) &amp; in(y,x) -&gt; in(z,x))). %22</v>
+      </c>
+      <c r="N91" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_22,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#22 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_22.proof}</v>
+      </c>
+      <c r="O91" s="14"/>
+      <c r="P91" s="14"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A92" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B92" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C92" s="14">
+        <v>23</v>
+      </c>
+      <c r="D92" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_23</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="3">
+        <v>600</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" s="3">
+        <v>600</v>
+      </c>
+      <c r="I92" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J92" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K92" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L92" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="15" t="str">
+        <f t="shared" si="30"/>
+        <v>(all q (plane(q) -&gt; (exists p (point(p) &amp; in(p,q))))). %23</v>
+      </c>
+      <c r="N92" s="15" t="str">
+        <f t="shared" si="26"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_23,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#23 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_23.proof}</v>
+      </c>
+      <c r="O92" s="14"/>
+      <c r="P92" s="14"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L69" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L86" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="23" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="10" day="30" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E18">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G18">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E35">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G35">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E52">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G52">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E69">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53:G69">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70:E92">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G70:G92">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4319,10 +5576,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996D9C58-6018-1D42-9792-6063C3F60A8A}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N105"/>
+  <dimension ref="A1:N119"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K117" sqref="K117"/>
+    <sheetView topLeftCell="K1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T120" sqref="T120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8650,7 +9907,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_14,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#14 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_14.proof}</v>
       </c>
     </row>
-    <row r="92" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="9">
         <v>43396</v>
       </c>
@@ -8699,7 +9956,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_1,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#1 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_1.proof}</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16">
         <v>43396</v>
       </c>
@@ -8748,7 +10005,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_2,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#2 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_2.proof}</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16">
         <v>43396</v>
       </c>
@@ -8797,7 +10054,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_3,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#3 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_3.proof}</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16">
         <v>43396</v>
       </c>
@@ -8846,7 +10103,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_4,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#4 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_4.proof}</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16">
         <v>43396</v>
       </c>
@@ -8895,7 +10152,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_5,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#5 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_5.proof}</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="16">
         <v>43396</v>
       </c>
@@ -8944,7 +10201,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_6,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#6 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_6.proof}</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="16">
         <v>43396</v>
       </c>
@@ -8993,7 +10250,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_7,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#7 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_7.proof}</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="16">
         <v>43396</v>
       </c>
@@ -9042,7 +10299,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_8,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#8 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_8.proof}</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="16">
         <v>43396</v>
       </c>
@@ -9091,7 +10348,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_9,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#9 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_9.proof}</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="16">
         <v>43396</v>
       </c>
@@ -9140,7 +10397,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_10,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#10 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_10.proof}</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="16">
         <v>43396</v>
       </c>
@@ -9189,7 +10446,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_11,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#11 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_11.proof}</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="16">
         <v>43396</v>
       </c>
@@ -9238,7 +10495,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_12,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#12 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_12.proof}</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="16">
         <v>43396</v>
       </c>
@@ -9287,109 +10544,761 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_13,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#13 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_13.proof}</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A105" s="16">
+    <row r="105" spans="1:14" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="17">
         <v>43396</v>
       </c>
-      <c r="B105" s="1" t="str">
+      <c r="B105" s="18" t="str">
         <f t="shared" si="27"/>
         <v>1023_most_graph2nonisolated_loopless</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="18">
         <v>14</v>
       </c>
-      <c r="D105" s="14" t="str">
+      <c r="D105" s="18" t="str">
         <f t="shared" si="24"/>
         <v>cycle_path_subgraph2most_group_14</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F105" s="3">
-        <v>60</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H105" s="3">
-        <v>60</v>
-      </c>
-      <c r="I105" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J105" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K105" s="14" t="str">
+      <c r="E105" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="20">
+        <v>60</v>
+      </c>
+      <c r="G105" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="20">
+        <v>60</v>
+      </c>
+      <c r="I105" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J105" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K105" s="18" t="str">
         <f t="shared" si="25"/>
         <v>cycle_path_subgraph2most_group</v>
       </c>
-      <c r="L105" s="15" t="s">
+      <c r="L105" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="M105" s="15" t="str">
+      <c r="M105" s="21" t="str">
         <f t="shared" si="28"/>
         <v>(all a1 all a2 all a3 all a4 all g all b1 all b2 all b3 (group(g) &amp; atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; mol(a1,g) &amp; mol(a2,g) &amp; mol(a3,g) &amp; mol(a4,g) &amp; bond(b1) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; bond(b2) &amp; mol(b2,g) &amp; mol(a1,b2) &amp; mol(a3,b2) &amp; bond(b3) &amp; mol(b3,g) &amp; mol(a1,b3) &amp; mol(a4,b3) -&gt; a4 = a3 | a2 = a3 | a4 = a2)). %14</v>
       </c>
-      <c r="N105" s="15" t="str">
+      <c r="N105" s="21" t="str">
         <f t="shared" si="26"/>
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_14,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#14 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_14.proof}</v>
       </c>
     </row>
+    <row r="106" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B106" s="14" t="str">
+        <f>TEXT(A106,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C106" s="14">
+        <v>1</v>
+      </c>
+      <c r="D106" s="14" t="str">
+        <f t="shared" ref="D106:D118" si="29">I106&amp;"2"&amp;J106&amp;"_"&amp;C106</f>
+        <v>cycle_path_subgraph_nonisolated2most_group_1</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="3">
+        <v>60</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H106" s="3">
+        <v>60</v>
+      </c>
+      <c r="I106" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J106" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K106" s="14" t="str">
+        <f t="shared" ref="K106:K118" si="30">I106&amp;"2"&amp;J106</f>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L106" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M106" s="15" t="str">
+        <f>L106&amp;" %"&amp;C106</f>
+        <v>(all x (atom(x) -&gt; -(bond(x) | group(x)))). %1</v>
+      </c>
+      <c r="N106" s="15" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D106&amp;",caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#"&amp;C106&amp;" in $T_{most\_group}$]{proofs/"&amp;D106&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_1,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#1 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_1.proof}</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A107" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B107" s="1" t="str">
+        <f t="shared" ref="B107:B118" si="31">TEXT(A107,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2</v>
+      </c>
+      <c r="D107" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_2</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="3">
+        <v>60</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H107" s="3">
+        <v>60</v>
+      </c>
+      <c r="I107" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J107" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K107" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L107" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M107" s="15" t="str">
+        <f t="shared" ref="M107:M118" si="32">L107&amp;" %"&amp;C107</f>
+        <v>(all x (bond(x) -&gt; -group(x))). %2</v>
+      </c>
+      <c r="N107" s="15" t="str">
+        <f t="shared" ref="N107:N118" si="33">"\lstinputlisting[style=p9proof,label="&amp;D107&amp;",caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#"&amp;C107&amp;" in $T_{most\_group}$]{proofs/"&amp;D107&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_2,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#2 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_2.proof}</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A108" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C108" s="1">
+        <v>3</v>
+      </c>
+      <c r="D108" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_3</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="3">
+        <v>60</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H108" s="3">
+        <v>60</v>
+      </c>
+      <c r="I108" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J108" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K108" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L108" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M108" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x all y (mol(x,y) &amp; group(x) &amp; group(y) -&gt; x = y)). %3</v>
+      </c>
+      <c r="N108" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_3,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#3 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_3.proof}</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A109" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C109" s="1">
+        <v>4</v>
+      </c>
+      <c r="D109" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_4</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" s="3">
+        <v>60</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H109" s="3">
+        <v>60</v>
+      </c>
+      <c r="I109" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J109" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K109" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L109" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M109" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x (group(x) -&gt; (exists a (atom(a) &amp; mol(a,x))))). %4</v>
+      </c>
+      <c r="N109" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_4,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#4 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_4.proof}</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A110" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C110" s="1">
+        <v>5</v>
+      </c>
+      <c r="D110" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_5</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="3">
+        <v>60</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H110" s="3">
+        <v>60</v>
+      </c>
+      <c r="I110" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J110" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K110" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L110" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M110" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x (atom(x) -&gt; (exists y (group(y) &amp; mol(x,y))))). %5</v>
+      </c>
+      <c r="N110" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_5,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#5 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_5.proof}</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A111" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C111" s="1">
+        <v>6</v>
+      </c>
+      <c r="D111" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_6</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" s="3">
+        <v>60</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H111" s="3">
+        <v>60</v>
+      </c>
+      <c r="I111" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J111" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K111" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L111" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M111" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x (atom(x) -&gt; (exists b exists y exists z (bond(b) &amp; group(y) &amp; atom(z) &amp; x != z &amp; mol(x,b) &amp; mol(z,b) &amp; mol(z,y))))). %6</v>
+      </c>
+      <c r="N111" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_6,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#6 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_6.proof}</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A112" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C112" s="1">
+        <v>7</v>
+      </c>
+      <c r="D112" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_7</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="3">
+        <v>60</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H112" s="3">
+        <v>60</v>
+      </c>
+      <c r="I112" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J112" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K112" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L112" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M112" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all b all g all x all y (atom(x) &amp; atom(y) &amp; x != y &amp; bond(b) &amp; group(g) &amp; mol(x,b) &amp; mol(y,b) &amp; mol(b,g) -&gt; mol(x,g))). %7</v>
+      </c>
+      <c r="N112" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_7,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#7 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_7.proof}</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A113" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C113" s="1">
+        <v>8</v>
+      </c>
+      <c r="D113" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_8</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="3">
+        <v>60</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H113" s="3">
+        <v>60</v>
+      </c>
+      <c r="I113" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J113" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K113" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L113" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M113" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x all y all z (atom(x) &amp; bond(y) &amp; group(z) &amp; mol(x,y) &amp; mol(y,z) -&gt; mol(x,z))). %8</v>
+      </c>
+      <c r="N113" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_8,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#8 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_8.proof}</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A114" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C114" s="1">
+        <v>9</v>
+      </c>
+      <c r="D114" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_9</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" s="3">
+        <v>60</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H114" s="3">
+        <v>60</v>
+      </c>
+      <c r="I114" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J114" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K114" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L114" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M114" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all y (group(y) -&gt; (exists x (atom(x) &amp; mol(x,y))))). %9</v>
+      </c>
+      <c r="N114" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_9,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#9 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_9.proof}</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C115" s="1">
+        <v>10</v>
+      </c>
+      <c r="D115" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_10</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" s="3">
+        <v>60</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H115" s="3">
+        <v>60</v>
+      </c>
+      <c r="I115" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J115" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K115" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L115" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M115" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x all y all b all g (atom(x) &amp; atom(y) &amp; bond(b) &amp; group(g) &amp; x != y &amp; mol(x,y) &amp; mol(y,g) &amp; mol(x,b) &amp; mol(y,b) -&gt; mol(b,g))). %10</v>
+      </c>
+      <c r="N115" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_10,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#10 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_10.proof}</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C116" s="1">
+        <v>11</v>
+      </c>
+      <c r="D116" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_11</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" s="3">
+        <v>60</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H116" s="3">
+        <v>60</v>
+      </c>
+      <c r="I116" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J116" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K116" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L116" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M116" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all b all g (bond(b) &amp; group(g) &amp; -mol(b,g) -&gt; (exists a (atom(a) &amp; mol(a,b) &amp; -mol(a,g))))). %11</v>
+      </c>
+      <c r="N116" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_11,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#11 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_11.proof}</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A117" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B117" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C117" s="1">
+        <v>12</v>
+      </c>
+      <c r="D117" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_12</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" s="3">
+        <v>60</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H117" s="3">
+        <v>60</v>
+      </c>
+      <c r="I117" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J117" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K117" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L117" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M117" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all x all y all z all w (group(x) &amp; end(y,x) &amp; end(z,x) &amp; end(w,x) -&gt; y = z | y = w | z = w)). %12</v>
+      </c>
+      <c r="N117" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_12,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#12 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_12.proof}</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A118" s="16">
+        <v>43403</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1030_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C118" s="1">
+        <v>13</v>
+      </c>
+      <c r="D118" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_13</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F118" s="3">
+        <v>60</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H118" s="3">
+        <v>60</v>
+      </c>
+      <c r="I118" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J118" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K118" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L118" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="M118" s="15" t="str">
+        <f t="shared" si="32"/>
+        <v>(all a1 all a2 all a3 all a4 all g all b1 all b2 all b3 (group(g) &amp; atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; mol(a1,g) &amp; mol(a2,g) &amp; mol(a3,g) &amp; mol(a4,g) &amp; bond(b1) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; bond(b2) &amp; mol(b2,g) &amp; mol(a1,b2) &amp; mol(a3,b2) &amp; bond(b3) &amp; mol(b3,g) &amp; mol(a1,b3) &amp; mol(a4,b3) -&gt; a4 = a3 | a2 = a3 | a4 = a2)). %13</v>
+      </c>
+      <c r="N118" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_13,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#13 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_13.proof}</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E119" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L105" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L118" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="23" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="10" day="30" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E49">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G49">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E63">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G50:G63">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E63">
+  <conditionalFormatting sqref="E64:E77">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G63">
+  <conditionalFormatting sqref="G64:G77">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:E77">
+  <conditionalFormatting sqref="E78:E91">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G64:G77">
+  <conditionalFormatting sqref="G78:G91">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78:E91">
+  <conditionalFormatting sqref="E92:E105">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G78:G91">
+  <conditionalFormatting sqref="G92:G105">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E92:E105">
+  <conditionalFormatting sqref="E106:E118">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92:G105">
+  <conditionalFormatting sqref="G106:G118">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated experiment spreadsheet for most
</commit_message>
<xml_diff>
--- a/ontologies/most/experiments/most_group_experiments.xlsx
+++ b/ontologies/most/experiments/most_group_experiments.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchui/Documents/GitHub/colore/ontologies/most/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFD857B-87F9-D943-AE09-7C2C6952ABF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E4AE78-6CBB-8D49-9E0B-9208BCB0E2C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="most_group2cycle_path_subgraph" sheetId="1" r:id="rId1"/>
     <sheet name="cycle_path_subgraph2most_group" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cycle_path_subgraph2most_group!$A$1:$L$118</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_group2cycle_path_subgraph!$A$1:$L$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cycle_path_subgraph2most_group!$A$1:$L$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">most_group2cycle_path_subgraph!$A$1:$L$110</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -225,9 +225,6 @@
     <t>cycle_path_subgraph_nonisolated</t>
   </si>
   <si>
-    <t>make sure to comment out definitions</t>
-  </si>
-  <si>
     <t>(all x all y all z all w all q all l1 all l2 all l3 (plane(q) &amp; point(x) &amp; point(y) &amp; point(z) &amp; point(w) &amp; in(x,q) &amp; in(y,q) &amp; in(z,q) &amp; in(w,q) &amp; line(l1) &amp; in(l1,q) &amp; in(x,l1) &amp; in(y,l1) &amp; line(l2) &amp; in(l2,q) &amp; in(x,l2) &amp; in(z,l2) &amp; line(l3) &amp; in(l3,q) &amp; in(x,l3) &amp; in(w,l3) -&gt; w = z | y = z | w = y)).</t>
   </si>
   <si>
@@ -244,6 +241,12 @@
   </si>
   <si>
     <t>(all p (point(p) -&gt; (exists q (plane(q) &amp; in(p,q))))).</t>
+  </si>
+  <si>
+    <t>prover9 goal</t>
+  </si>
+  <si>
+    <t>Prover9 Goal</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,31 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1025,10 +1052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P98" sqref="P98"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1086,6 +1113,9 @@
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="M1" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="N1" s="6" t="s">
         <v>21</v>
       </c>
@@ -4371,7 +4401,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph}$]{proofs/most_group2cycle_path_subgraph_17.proof}</v>
       </c>
     </row>
-    <row r="70" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16">
         <v>43403</v>
       </c>
@@ -4409,7 +4439,7 @@
         <v>most_group2cycle_path_subgraph_nonisolated</v>
       </c>
       <c r="L70" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M70" s="15" t="str">
         <f t="shared" ref="M70:M86" si="22">L70&amp;" %"&amp;C70</f>
@@ -4420,7 +4450,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_1,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#1 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_1.proof}</v>
       </c>
     </row>
-    <row r="71" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16">
         <v>43403</v>
       </c>
@@ -4458,7 +4488,7 @@
         <v>most_group2cycle_path_subgraph_nonisolated</v>
       </c>
       <c r="L71" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M71" s="15" t="str">
         <f t="shared" si="22"/>
@@ -4469,7 +4499,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_2,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#2 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_2.proof}</v>
       </c>
     </row>
-    <row r="72" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16">
         <v>43403</v>
       </c>
@@ -4507,7 +4537,7 @@
         <v>most_group2cycle_path_subgraph_nonisolated</v>
       </c>
       <c r="L72" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M72" s="15" t="str">
         <f t="shared" si="22"/>
@@ -4518,7 +4548,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_3,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#3 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_3.proof}</v>
       </c>
     </row>
-    <row r="73" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16">
         <v>43403</v>
       </c>
@@ -4556,7 +4586,7 @@
         <v>most_group2cycle_path_subgraph_nonisolated</v>
       </c>
       <c r="L73" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M73" s="15" t="str">
         <f t="shared" si="22"/>
@@ -4567,7 +4597,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_4,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#4 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_4.proof}</v>
       </c>
     </row>
-    <row r="74" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16">
         <v>43403</v>
       </c>
@@ -4605,7 +4635,7 @@
         <v>most_group2cycle_path_subgraph_nonisolated</v>
       </c>
       <c r="L74" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M74" s="15" t="str">
         <f t="shared" si="22"/>
@@ -4616,7 +4646,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_5,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#5 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_5.proof}</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16">
         <v>43403</v>
       </c>
@@ -4665,7 +4695,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_6,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#6 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_6.proof}</v>
       </c>
     </row>
-    <row r="76" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16">
         <v>43403</v>
       </c>
@@ -4714,7 +4744,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_7,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#7 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_7.proof}</v>
       </c>
     </row>
-    <row r="77" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16">
         <v>43403</v>
       </c>
@@ -4763,7 +4793,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_8,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#8 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_8.proof}</v>
       </c>
     </row>
-    <row r="78" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16">
         <v>43403</v>
       </c>
@@ -4812,7 +4842,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_9,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#9 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_9.proof}</v>
       </c>
     </row>
-    <row r="79" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16">
         <v>43403</v>
       </c>
@@ -4861,7 +4891,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_10,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#10 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_10.proof}</v>
       </c>
     </row>
-    <row r="80" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16">
         <v>43403</v>
       </c>
@@ -4910,7 +4940,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_11,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#11 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_11.proof}</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
         <v>43403</v>
       </c>
@@ -4959,7 +4989,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_12,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#12 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_12.proof}</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16">
         <v>43403</v>
       </c>
@@ -5008,7 +5038,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_13,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#13 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_13.proof}</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
         <v>43403</v>
       </c>
@@ -5057,7 +5087,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_14,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#14 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_14.proof}</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16">
         <v>43403</v>
       </c>
@@ -5106,7 +5136,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_15,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#15 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_15.proof}</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16">
         <v>43403</v>
       </c>
@@ -5155,7 +5185,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_16,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#16 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_16.proof}</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16">
         <v>43403</v>
       </c>
@@ -5204,7 +5234,7 @@
         <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_17.proof}</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16">
         <v>43403</v>
       </c>
@@ -5255,7 +5285,7 @@
       <c r="O87" s="14"/>
       <c r="P87" s="14"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16">
         <v>43403</v>
       </c>
@@ -5293,7 +5323,7 @@
         <v>most_group2cycle_path_subgraph_nonisolated</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M88" s="15" t="str">
         <f t="shared" si="30"/>
@@ -5306,7 +5336,7 @@
       <c r="O88" s="14"/>
       <c r="P88" s="14"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16">
         <v>43403</v>
       </c>
@@ -5357,7 +5387,7 @@
       <c r="O89" s="14"/>
       <c r="P89" s="14"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16">
         <v>43403</v>
       </c>
@@ -5408,7 +5438,7 @@
       <c r="O90" s="14"/>
       <c r="P90" s="14"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16">
         <v>43403</v>
       </c>
@@ -5459,7 +5489,7 @@
       <c r="O91" s="14"/>
       <c r="P91" s="14"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16">
         <v>43403</v>
       </c>
@@ -5510,61 +5540,979 @@
       <c r="O92" s="14"/>
       <c r="P92" s="14"/>
     </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A93" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B93" s="14" t="str">
+        <f>TEXT(A93,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C93" s="14">
+        <v>1</v>
+      </c>
+      <c r="D93" s="14" t="str">
+        <f t="shared" ref="D93:D110" si="31">I93&amp;"2"&amp;J93&amp;"_"&amp;C93</f>
+        <v>most_group2cycle_path_subgraph_nonisolated_1</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="3">
+        <v>600</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" s="3">
+        <v>600</v>
+      </c>
+      <c r="I93" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K93" s="14" t="str">
+        <f t="shared" ref="K93:K110" si="32">I93&amp;"2"&amp;J93</f>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L93" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M93" s="15" t="str">
+        <f t="shared" ref="M93:M110" si="33">L93&amp;" %"&amp;C93</f>
+        <v>(all x all y all z all w all q all l1 all l2 all l3 (plane(q) &amp; point(x) &amp; point(y) &amp; point(z) &amp; point(w) &amp; in(x,q) &amp; in(y,q) &amp; in(z,q) &amp; in(w,q) &amp; line(l1) &amp; in(l1,q) &amp; in(x,l1) &amp; in(y,l1) &amp; line(l2) &amp; in(l2,q) &amp; in(x,l2) &amp; in(z,l2) &amp; line(l3) &amp; in(l3,q) &amp; in(x,l3) &amp; in(w,l3) -&gt; w = z | y = z | w = y)). %1</v>
+      </c>
+      <c r="N93" s="15" t="str">
+        <f t="shared" ref="N93:N110" si="34">"\lstinputlisting[style=p9proof,label="&amp;D93&amp;",caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#"&amp;C93&amp;" in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/"&amp;D93&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_1,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#1 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_1.proof}</v>
+      </c>
+      <c r="O93" s="14"/>
+      <c r="P93" s="14"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A94" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B94" s="14" t="str">
+        <f t="shared" ref="B94:B110" si="35">TEXT(A94,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C94" s="14">
+        <v>2</v>
+      </c>
+      <c r="D94" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_2</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="3">
+        <v>600</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" s="3">
+        <v>600</v>
+      </c>
+      <c r="I94" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L94" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M94" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all q all x all y all z (planar_pendant(x,q) &amp; planar_pendant(y,q) &amp; planar_pendant(z,q) -&gt; x = y | y = z | z = x)). %2</v>
+      </c>
+      <c r="N94" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_2,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#2 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_2.proof}</v>
+      </c>
+      <c r="O94" s="14"/>
+      <c r="P94" s="14"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A95" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B95" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C95" s="14">
+        <v>3</v>
+      </c>
+      <c r="D95" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_3</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="3">
+        <v>600</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" s="3">
+        <v>600</v>
+      </c>
+      <c r="I95" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J95" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L95" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M95" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all p (point(p) -&gt; (exists l (line(l) &amp; in(p,l))))). %3</v>
+      </c>
+      <c r="N95" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_3,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#3 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_3.proof}</v>
+      </c>
+      <c r="O95" s="14"/>
+      <c r="P95" s="14"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A96" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B96" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C96" s="14">
+        <v>4</v>
+      </c>
+      <c r="D96" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_4</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="3">
+        <v>600</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" s="3">
+        <v>600</v>
+      </c>
+      <c r="I96" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J96" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L96" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M96" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all l all q (line(l) &amp; plane(q) &amp; -in(l,q) -&gt; (exists p (point(p) &amp; in(p,l) &amp; -in(p,q))))). %4</v>
+      </c>
+      <c r="N96" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_4,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#4 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_4.proof}</v>
+      </c>
+      <c r="O96" s="14"/>
+      <c r="P96" s="14"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A97" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B97" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C97" s="14">
+        <v>5</v>
+      </c>
+      <c r="D97" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_5</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97" s="3">
+        <v>600</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" s="3">
+        <v>600</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J97" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L97" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M97" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all l (line(l) -&gt; (exists x exists y (point(x) &amp; point(y) &amp; x != y &amp; in(x,l) &amp; in(y,l))))). %5</v>
+      </c>
+      <c r="N97" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_5,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#5 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_5.proof}</v>
+      </c>
+      <c r="O97" s="14"/>
+      <c r="P97" s="14"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A98" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B98" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C98" s="14">
+        <v>6</v>
+      </c>
+      <c r="D98" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_6</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="3">
+        <v>600</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" s="3">
+        <v>600</v>
+      </c>
+      <c r="I98" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J98" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L98" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M98" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x all y (in(x,y) -&gt; in(y,x))). %6</v>
+      </c>
+      <c r="N98" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_6,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#6 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_6.proof}</v>
+      </c>
+      <c r="O98" s="14"/>
+      <c r="P98" s="14"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A99" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B99" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C99" s="14">
+        <v>7</v>
+      </c>
+      <c r="D99" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_7</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="3">
+        <v>600</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" s="3">
+        <v>600</v>
+      </c>
+      <c r="I99" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J99" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L99" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M99" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x (point(x) | line(x) | plane(x) -&gt; in(x,x))). %7</v>
+      </c>
+      <c r="N99" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_7,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#7 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_7.proof}</v>
+      </c>
+      <c r="O99" s="14"/>
+      <c r="P99" s="14"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A100" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B100" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C100" s="14">
+        <v>8</v>
+      </c>
+      <c r="D100" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_8</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" s="3">
+        <v>600</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" s="3">
+        <v>600</v>
+      </c>
+      <c r="I100" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J100" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L100" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M100" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all p (point(p) -&gt; -line(p))). %8</v>
+      </c>
+      <c r="N100" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_8,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#8 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_8.proof}</v>
+      </c>
+      <c r="O100" s="14"/>
+      <c r="P100" s="14"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A101" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B101" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C101" s="14">
+        <v>9</v>
+      </c>
+      <c r="D101" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_9</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="3">
+        <v>600</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="3">
+        <v>600</v>
+      </c>
+      <c r="I101" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L101" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M101" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all p (point(p) -&gt; -plane(p))). %9</v>
+      </c>
+      <c r="N101" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_9,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#9 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_9.proof}</v>
+      </c>
+      <c r="O101" s="14"/>
+      <c r="P101" s="14"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A102" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B102" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C102" s="14">
+        <v>10</v>
+      </c>
+      <c r="D102" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_10</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="3">
+        <v>600</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H102" s="3">
+        <v>600</v>
+      </c>
+      <c r="I102" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J102" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L102" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M102" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all p (plane(p) -&gt; -line(p))). %10</v>
+      </c>
+      <c r="N102" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_10,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#10 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_10.proof}</v>
+      </c>
+      <c r="O102" s="14"/>
+      <c r="P102" s="14"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A103" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B103" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C103" s="14">
+        <v>11</v>
+      </c>
+      <c r="D103" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_11</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" s="3">
+        <v>600</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="3">
+        <v>600</v>
+      </c>
+      <c r="I103" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J103" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L103" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M103" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x all y (in(x,y) &amp; point(x) &amp; point(y) -&gt; x = y)). %11</v>
+      </c>
+      <c r="N103" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_11,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#11 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_11.proof}</v>
+      </c>
+      <c r="O103" s="14"/>
+      <c r="P103" s="14"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A104" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B104" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C104" s="14">
+        <v>12</v>
+      </c>
+      <c r="D104" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_12</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" s="3">
+        <v>600</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" s="3">
+        <v>600</v>
+      </c>
+      <c r="I104" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J104" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L104" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M104" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x all y (in(x,y) &amp; line(x) &amp; line(y) -&gt; x = y)). %12</v>
+      </c>
+      <c r="N104" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_12,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#12 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_12.proof}</v>
+      </c>
+      <c r="O104" s="14"/>
+      <c r="P104" s="14"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A105" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B105" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C105" s="14">
+        <v>13</v>
+      </c>
+      <c r="D105" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_13</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="3">
+        <v>600</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="3">
+        <v>600</v>
+      </c>
+      <c r="I105" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J105" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K105" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L105" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M105" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x all y (in(x,y) &amp; plane(x) &amp; plane(y) -&gt; x = y)). %13</v>
+      </c>
+      <c r="N105" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_13,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#13 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_13.proof}</v>
+      </c>
+      <c r="O105" s="14"/>
+      <c r="P105" s="14"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A106" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B106" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C106" s="14">
+        <v>14</v>
+      </c>
+      <c r="D106" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_14</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="3">
+        <v>600</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H106" s="3">
+        <v>600</v>
+      </c>
+      <c r="I106" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J106" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K106" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L106" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="M106" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all p (point(p) -&gt; (exists q (plane(q) &amp; in(p,q))))). %14</v>
+      </c>
+      <c r="N106" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_14,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#14 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_14.proof}</v>
+      </c>
+      <c r="O106" s="14"/>
+      <c r="P106" s="14"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A107" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B107" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C107" s="14">
+        <v>15</v>
+      </c>
+      <c r="D107" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_15</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="3">
+        <v>600</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H107" s="3">
+        <v>600</v>
+      </c>
+      <c r="I107" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J107" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K107" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L107" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M107" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all l (line(l) -&gt; (exists x (point(x) &amp; in(x,l))))). %15</v>
+      </c>
+      <c r="N107" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_15,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#15 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_15.proof}</v>
+      </c>
+      <c r="O107" s="14"/>
+      <c r="P107" s="14"/>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A108" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B108" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C108" s="14">
+        <v>16</v>
+      </c>
+      <c r="D108" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_16</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="3">
+        <v>600</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H108" s="3">
+        <v>600</v>
+      </c>
+      <c r="I108" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J108" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K108" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L108" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M108" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x all y all z all l (point(x) &amp; point(y) &amp; point(z) &amp; line(l) &amp; in(x,l) &amp; in(y,l) &amp; in(z,l) -&gt; z = x | z = y | x = y)). %16</v>
+      </c>
+      <c r="N108" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_16,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#16 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_16.proof}</v>
+      </c>
+      <c r="O108" s="14"/>
+      <c r="P108" s="14"/>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A109" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B109" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C109" s="14">
+        <v>17</v>
+      </c>
+      <c r="D109" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_17</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" s="3">
+        <v>600</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H109" s="3">
+        <v>600</v>
+      </c>
+      <c r="I109" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J109" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K109" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L109" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M109" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all x all y all z (plane(x) &amp; line(y) &amp; point(z) &amp; in(z,y) &amp; in(y,x) -&gt; in(z,x))). %17</v>
+      </c>
+      <c r="N109" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_17,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#17 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_17.proof}</v>
+      </c>
+      <c r="O109" s="14"/>
+      <c r="P109" s="14"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A110" s="7">
+        <v>43412</v>
+      </c>
+      <c r="B110" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C110" s="14">
+        <v>18</v>
+      </c>
+      <c r="D110" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>most_group2cycle_path_subgraph_nonisolated_18</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="3">
+        <v>600</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H110" s="3">
+        <v>600</v>
+      </c>
+      <c r="I110" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J110" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K110" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>most_group2cycle_path_subgraph_nonisolated</v>
+      </c>
+      <c r="L110" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M110" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v>(all q (plane(q) -&gt; (exists p (point(p) &amp; in(p,q))))). %18</v>
+      </c>
+      <c r="N110" s="15" t="str">
+        <f t="shared" si="34"/>
+        <v>\lstinputlisting[style=p9proof,label=most_group2cycle_path_subgraph_nonisolated_18,caption=$T_{most\_group} \cup \Delta_2 \models$ Axiom \#18 in $T_{cycle\_path\_subgraph\_nonisolated}$]{proofs/most_group2cycle_path_subgraph_nonisolated_18.proof}</v>
+      </c>
+      <c r="O110" s="14"/>
+      <c r="P110" s="14"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L86" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L110" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="30" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="11" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E18">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G18">
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E35">
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G35">
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E52">
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G52">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E69">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53:G69">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70:E92">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+  <conditionalFormatting sqref="E70:E110">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G70:G92">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+  <conditionalFormatting sqref="G70:G110">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5576,10 +6524,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996D9C58-6018-1D42-9792-6063C3F60A8A}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:N131"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T120" sqref="T120"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L140" sqref="L140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5637,6 +6585,9 @@
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="M1" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="N1" s="6" t="s">
         <v>21</v>
       </c>
@@ -10593,7 +11544,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph2most_group_14,caption=$T_{cycle\_path\_subgraph} \cup \Pi_2 \models$ Axiom \#14 in $T_{most\_group}$]{proofs/cycle_path_subgraph2most_group_14.proof}</v>
       </c>
     </row>
-    <row r="106" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="16">
         <v>43403</v>
       </c>
@@ -10642,7 +11593,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_1,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#1 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_1.proof}</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="16">
         <v>43403</v>
       </c>
@@ -10691,7 +11642,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_2,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#2 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_2.proof}</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="16">
         <v>43403</v>
       </c>
@@ -10740,7 +11691,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_3,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#3 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_3.proof}</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="16">
         <v>43403</v>
       </c>
@@ -10789,7 +11740,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_4,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#4 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_4.proof}</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="16">
         <v>43403</v>
       </c>
@@ -10838,7 +11789,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_5,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#5 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_5.proof}</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="16">
         <v>43403</v>
       </c>
@@ -10887,7 +11838,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_6,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#6 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_6.proof}</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="16">
         <v>43403</v>
       </c>
@@ -10936,7 +11887,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_7,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#7 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_7.proof}</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="16">
         <v>43403</v>
       </c>
@@ -10985,7 +11936,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_8,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#8 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_8.proof}</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="16">
         <v>43403</v>
       </c>
@@ -11034,7 +11985,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_9,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#9 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_9.proof}</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="16">
         <v>43403</v>
       </c>
@@ -11083,7 +12034,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_10,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#10 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_10.proof}</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="16">
         <v>43403</v>
       </c>
@@ -11132,7 +12083,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_11,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#11 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_11.proof}</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="16">
         <v>43403</v>
       </c>
@@ -11181,7 +12132,7 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_12,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#12 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_12.proof}</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="16">
         <v>43403</v>
       </c>
@@ -11230,75 +12181,717 @@
         <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_13,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#13 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_13.proof}</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E119" s="1" t="s">
-        <v>66</v>
+    <row r="119" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B119" s="14" t="str">
+        <f>TEXT(A119,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C119" s="14">
+        <v>1</v>
+      </c>
+      <c r="D119" s="14" t="str">
+        <f t="shared" ref="D119:D131" si="34">I119&amp;"2"&amp;J119&amp;"_"&amp;C119</f>
+        <v>cycle_path_subgraph_nonisolated2most_group_1</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119" s="3">
+        <v>600</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H119" s="3">
+        <v>60</v>
+      </c>
+      <c r="I119" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J119" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K119" s="14" t="str">
+        <f t="shared" ref="K119:K131" si="35">I119&amp;"2"&amp;J119</f>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L119" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M119" s="15" t="str">
+        <f>L119&amp;" %"&amp;C119</f>
+        <v>(all x (atom(x) -&gt; -(bond(x) | group(x)))). %1</v>
+      </c>
+      <c r="N119" s="15" t="str">
+        <f>"\lstinputlisting[style=p9proof,label="&amp;D119&amp;",caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#"&amp;C119&amp;" in $T_{most\_group}$]{proofs/"&amp;D119&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_1,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#1 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_1.proof}</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B120" s="1" t="str">
+        <f t="shared" ref="B120:B131" si="36">TEXT(A120,"mmdd")&amp;"_most_graph2nonisolated_loopless"</f>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C120" s="1">
+        <v>2</v>
+      </c>
+      <c r="D120" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_2</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F120" s="3">
+        <v>600</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H120" s="3">
+        <v>60</v>
+      </c>
+      <c r="I120" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J120" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K120" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L120" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M120" s="15" t="str">
+        <f t="shared" ref="M120:M131" si="37">L120&amp;" %"&amp;C120</f>
+        <v>(all x (bond(x) -&gt; -group(x))). %2</v>
+      </c>
+      <c r="N120" s="15" t="str">
+        <f t="shared" ref="N120:N131" si="38">"\lstinputlisting[style=p9proof,label="&amp;D120&amp;",caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#"&amp;C120&amp;" in $T_{most\_group}$]{proofs/"&amp;D120&amp;".proof}"</f>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_2,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#2 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_2.proof}</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B121" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C121" s="1">
+        <v>3</v>
+      </c>
+      <c r="D121" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_3</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121" s="3">
+        <v>600</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H121" s="3">
+        <v>60</v>
+      </c>
+      <c r="I121" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J121" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K121" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L121" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M121" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x all y (mol(x,y) &amp; group(x) &amp; group(y) -&gt; x = y)). %3</v>
+      </c>
+      <c r="N121" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_3,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#3 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_3.proof}</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A122" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B122" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C122" s="1">
+        <v>4</v>
+      </c>
+      <c r="D122" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_4</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F122" s="3">
+        <v>600</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H122" s="3">
+        <v>60</v>
+      </c>
+      <c r="I122" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J122" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K122" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L122" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M122" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x (group(x) -&gt; (exists a (atom(a) &amp; mol(a,x))))). %4</v>
+      </c>
+      <c r="N122" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_4,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#4 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_4.proof}</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A123" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B123" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C123" s="1">
+        <v>5</v>
+      </c>
+      <c r="D123" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_5</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="3">
+        <v>600</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H123" s="3">
+        <v>60</v>
+      </c>
+      <c r="I123" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J123" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K123" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L123" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M123" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x (atom(x) -&gt; (exists y (group(y) &amp; mol(x,y))))). %5</v>
+      </c>
+      <c r="N123" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_5,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#5 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_5.proof}</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A124" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B124" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C124" s="1">
+        <v>6</v>
+      </c>
+      <c r="D124" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_6</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F124" s="3">
+        <v>600</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H124" s="3">
+        <v>60</v>
+      </c>
+      <c r="I124" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J124" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K124" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L124" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M124" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x (atom(x) -&gt; (exists b exists y exists z (bond(b) &amp; group(y) &amp; atom(z) &amp; x != z &amp; mol(x,b) &amp; mol(z,b) &amp; mol(z,y))))). %6</v>
+      </c>
+      <c r="N124" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_6,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#6 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_6.proof}</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A125" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B125" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C125" s="1">
+        <v>7</v>
+      </c>
+      <c r="D125" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_7</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125" s="3">
+        <v>600</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H125" s="3">
+        <v>60</v>
+      </c>
+      <c r="I125" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J125" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K125" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L125" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M125" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all b all g all x all y (atom(x) &amp; atom(y) &amp; x != y &amp; bond(b) &amp; group(g) &amp; mol(x,b) &amp; mol(y,b) &amp; mol(b,g) -&gt; mol(x,g))). %7</v>
+      </c>
+      <c r="N125" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_7,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#7 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_7.proof}</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A126" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B126" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C126" s="1">
+        <v>8</v>
+      </c>
+      <c r="D126" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_8</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="3">
+        <v>600</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H126" s="3">
+        <v>60</v>
+      </c>
+      <c r="I126" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J126" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K126" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L126" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M126" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x all y all z (atom(x) &amp; bond(y) &amp; group(z) &amp; mol(x,y) &amp; mol(y,z) -&gt; mol(x,z))). %8</v>
+      </c>
+      <c r="N126" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_8,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#8 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_8.proof}</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B127" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C127" s="1">
+        <v>9</v>
+      </c>
+      <c r="D127" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_9</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F127" s="3">
+        <v>600</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H127" s="3">
+        <v>60</v>
+      </c>
+      <c r="I127" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J127" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K127" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L127" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M127" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all y (group(y) -&gt; (exists x (atom(x) &amp; mol(x,y))))). %9</v>
+      </c>
+      <c r="N127" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_9,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#9 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_9.proof}</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A128" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B128" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C128" s="1">
+        <v>10</v>
+      </c>
+      <c r="D128" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_10</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F128" s="3">
+        <v>600</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H128" s="3">
+        <v>60</v>
+      </c>
+      <c r="I128" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J128" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K128" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L128" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M128" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x all y all b all g (atom(x) &amp; atom(y) &amp; bond(b) &amp; group(g) &amp; x != y &amp; mol(x,y) &amp; mol(y,g) &amp; mol(x,b) &amp; mol(y,b) -&gt; mol(b,g))). %10</v>
+      </c>
+      <c r="N128" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_10,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#10 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_10.proof}</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A129" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B129" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C129" s="1">
+        <v>11</v>
+      </c>
+      <c r="D129" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_11</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F129" s="3">
+        <v>600</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H129" s="3">
+        <v>60</v>
+      </c>
+      <c r="I129" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J129" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K129" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L129" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M129" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all b all g (bond(b) &amp; group(g) &amp; -mol(b,g) -&gt; (exists a (atom(a) &amp; mol(a,b) &amp; -mol(a,g))))). %11</v>
+      </c>
+      <c r="N129" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_11,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#11 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_11.proof}</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A130" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B130" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C130" s="1">
+        <v>12</v>
+      </c>
+      <c r="D130" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_12</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130" s="3">
+        <v>600</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H130" s="3">
+        <v>60</v>
+      </c>
+      <c r="I130" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J130" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K130" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L130" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M130" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all x all y all z all w (group(x) &amp; end(y,x) &amp; end(z,x) &amp; end(w,x) -&gt; y = z | y = w | z = w)). %12</v>
+      </c>
+      <c r="N130" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_12,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#12 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_12.proof}</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A131" s="16">
+        <v>43412</v>
+      </c>
+      <c r="B131" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1108_most_graph2nonisolated_loopless</v>
+      </c>
+      <c r="C131" s="1">
+        <v>13</v>
+      </c>
+      <c r="D131" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>cycle_path_subgraph_nonisolated2most_group_13</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F131" s="3">
+        <v>600</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H131" s="3">
+        <v>60</v>
+      </c>
+      <c r="I131" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J131" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K131" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>cycle_path_subgraph_nonisolated2most_group</v>
+      </c>
+      <c r="L131" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="M131" s="15" t="str">
+        <f t="shared" si="37"/>
+        <v>(all a1 all a2 all a3 all a4 all g all b1 all b2 all b3 (group(g) &amp; atom(a1) &amp; atom(a2) &amp; atom(a3) &amp; atom(a4) &amp; mol(a1,g) &amp; mol(a2,g) &amp; mol(a3,g) &amp; mol(a4,g) &amp; bond(b1) &amp; mol(b1,g) &amp; mol(a1,b1) &amp; mol(a2,b1) &amp; bond(b2) &amp; mol(b2,g) &amp; mol(a1,b2) &amp; mol(a3,b2) &amp; bond(b3) &amp; mol(b3,g) &amp; mol(a1,b3) &amp; mol(a4,b3) -&gt; a4 = a3 | a2 = a3 | a4 = a2)). %13</v>
+      </c>
+      <c r="N131" s="15" t="str">
+        <f t="shared" si="38"/>
+        <v>\lstinputlisting[style=p9proof,label=cycle_path_subgraph_nonisolated2most_group_13,caption=$T_{cycle\_path\_subgraph\_nonisolated} \cup \Pi_2 \models$ Axiom \#13 in $T_{most\_group}$]{proofs/cycle_path_subgraph_nonisolated2most_group_13.proof}</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L118" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L131" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2018" month="10" day="30" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="11" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E2:E49">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G49">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E63">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G50:G63">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E63">
+  <conditionalFormatting sqref="E64:E77">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G63">
+  <conditionalFormatting sqref="G64:G77">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:E77">
+  <conditionalFormatting sqref="E78:E91">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G64:G77">
+  <conditionalFormatting sqref="G78:G91">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78:E91">
+  <conditionalFormatting sqref="E92:E105">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G78:G91">
+  <conditionalFormatting sqref="G92:G105">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E92:E105">
+  <conditionalFormatting sqref="E106:E118">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92:G105">
+  <conditionalFormatting sqref="G106:G118">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106:E118">
+  <conditionalFormatting sqref="E119:E131">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G106:G118">
+  <conditionalFormatting sqref="G119:G131">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>